<commit_message>
Update state survey file
</commit_message>
<xml_diff>
--- a/statistics_files/2023/99.year.end/2023.state.survey.xlsx
+++ b/statistics_files/2023/99.year.end/2023.state.survey.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\GitHub\next_statistics\statistics_files\2023\99.year.end\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BDE62F5-5024-449F-B741-BB0D2DE3D618}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EDBF630-AE39-457D-AAFA-2085F6BADEAA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11295" tabRatio="717" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,14 +28,14 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'State Survey-2020 data'!$A$1:$N$57</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'State Survey-2021 data'!$A$1:$M$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'State Survey-2022 data'!$A$1:$M$55</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'State Survey-2023 data'!$A$1:$M$58</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'State Survey-2023 data'!$A$1:$N$58</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="170">
   <si>
     <t>branchcode</t>
   </si>
@@ -544,6 +544,9 @@
   </si>
   <si>
     <t>Question 9.4 - total of all other materials at end of 2023</t>
+  </si>
+  <si>
+    <t>Question 10.6a - provide annual circulation for WIFI hotspots</t>
   </si>
 </sst>
 </file>
@@ -1215,16 +1218,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFCCFF"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -1505,7 +1499,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AA5473C-0C90-44FF-9C47-2BBE3539FF34}">
-  <dimension ref="A1:M59"/>
+  <dimension ref="A1:N59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -1517,10 +1511,10 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.7109375" style="7" customWidth="1"/>
-    <col min="2" max="13" width="16.7109375" style="7" customWidth="1"/>
+    <col min="2" max="14" width="16.7109375" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="8" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="8" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
@@ -1546,22 +1540,25 @@
         <v>168</v>
       </c>
       <c r="I1" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="J1" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="J1" s="24" t="s">
+      <c r="K1" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="K1" s="24" t="s">
+      <c r="L1" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="L1" s="24" t="s">
+      <c r="M1" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="M1" s="24" t="s">
+      <c r="N1" s="24" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>106</v>
       </c>
@@ -1587,22 +1584,25 @@
         <v>1414</v>
       </c>
       <c r="I2" s="1">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1">
         <v>34429</v>
       </c>
-      <c r="J2" s="1">
+      <c r="K2" s="1">
         <v>37031</v>
       </c>
-      <c r="K2" s="14">
+      <c r="L2" s="14">
         <v>1462</v>
       </c>
-      <c r="L2" s="1">
+      <c r="M2" s="1">
         <v>11009</v>
       </c>
-      <c r="M2" s="1">
+      <c r="N2" s="1">
         <v>12393</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>107</v>
       </c>
@@ -1628,22 +1628,25 @@
         <v>608</v>
       </c>
       <c r="I3" s="2">
+        <v>60</v>
+      </c>
+      <c r="J3" s="2">
         <v>15036</v>
       </c>
-      <c r="J3" s="2">
+      <c r="K3" s="2">
         <v>18825</v>
       </c>
-      <c r="K3" s="15">
+      <c r="L3" s="15">
         <v>1127</v>
       </c>
-      <c r="L3" s="2">
+      <c r="M3" s="2">
         <v>4354</v>
       </c>
-      <c r="M3" s="2">
+      <c r="N3" s="2">
         <v>4376</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>108</v>
       </c>
@@ -1669,22 +1672,25 @@
         <v>939</v>
       </c>
       <c r="I4" s="1">
+        <v>34</v>
+      </c>
+      <c r="J4" s="1">
         <v>48424</v>
       </c>
-      <c r="J4" s="1">
+      <c r="K4" s="1">
         <v>70073</v>
       </c>
-      <c r="K4" s="14">
+      <c r="L4" s="14">
         <v>3814</v>
       </c>
-      <c r="L4" s="1">
+      <c r="M4" s="1">
         <v>11464</v>
       </c>
-      <c r="M4" s="1">
+      <c r="N4" s="1">
         <v>10633</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
         <v>109</v>
       </c>
@@ -1710,22 +1716,25 @@
         <v>83</v>
       </c>
       <c r="I5" s="2">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2">
         <v>1176</v>
       </c>
-      <c r="J5" s="2">
+      <c r="K5" s="2">
         <v>1263</v>
       </c>
-      <c r="K5" s="15">
+      <c r="L5" s="15">
         <v>1</v>
       </c>
-      <c r="L5" s="2">
+      <c r="M5" s="2">
         <v>1098</v>
       </c>
-      <c r="M5" s="2">
+      <c r="N5" s="2">
         <v>267</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>110</v>
       </c>
@@ -1751,22 +1760,25 @@
         <v>1686</v>
       </c>
       <c r="I6" s="1">
+        <v>59</v>
+      </c>
+      <c r="J6" s="1">
         <v>29178</v>
       </c>
-      <c r="J6" s="1">
+      <c r="K6" s="1">
         <v>40691</v>
       </c>
-      <c r="K6" s="14">
+      <c r="L6" s="14">
         <v>3201</v>
       </c>
-      <c r="L6" s="1">
+      <c r="M6" s="1">
         <v>13217</v>
       </c>
-      <c r="M6" s="1">
+      <c r="N6" s="1">
         <v>10303</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
         <v>111</v>
       </c>
@@ -1792,22 +1804,25 @@
         <v>231</v>
       </c>
       <c r="I7" s="2">
+        <v>171</v>
+      </c>
+      <c r="J7" s="2">
         <v>4785</v>
       </c>
-      <c r="J7" s="2">
+      <c r="K7" s="2">
         <v>2891</v>
       </c>
-      <c r="K7" s="15">
+      <c r="L7" s="15">
         <v>1334</v>
       </c>
-      <c r="L7" s="2">
+      <c r="M7" s="2">
         <v>2168</v>
       </c>
-      <c r="M7" s="2">
+      <c r="N7" s="2">
         <v>1753</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>112</v>
       </c>
@@ -1833,22 +1848,25 @@
         <v>28</v>
       </c>
       <c r="I8" s="1">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1">
         <v>5938</v>
       </c>
-      <c r="J8" s="1">
+      <c r="K8" s="1">
         <v>3310</v>
       </c>
-      <c r="K8" s="14">
+      <c r="L8" s="14">
         <v>54</v>
       </c>
-      <c r="L8" s="1">
+      <c r="M8" s="1">
         <v>1832</v>
       </c>
-      <c r="M8" s="1">
+      <c r="N8" s="1">
         <v>1016</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
         <v>113</v>
       </c>
@@ -1874,22 +1892,25 @@
         <v>36</v>
       </c>
       <c r="I9" s="2">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2">
         <v>2189</v>
       </c>
-      <c r="J9" s="2">
+      <c r="K9" s="2">
         <v>1271</v>
       </c>
-      <c r="K9" s="15">
+      <c r="L9" s="15">
         <v>18</v>
       </c>
-      <c r="L9" s="2">
+      <c r="M9" s="2">
         <v>684</v>
       </c>
-      <c r="M9" s="2">
+      <c r="N9" s="2">
         <v>445</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>114</v>
       </c>
@@ -1915,22 +1936,25 @@
         <v>4</v>
       </c>
       <c r="I10" s="1">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1">
         <v>142</v>
       </c>
-      <c r="J10" s="1">
+      <c r="K10" s="1">
         <v>331</v>
       </c>
-      <c r="K10" s="14">
-        <v>0</v>
-      </c>
-      <c r="L10" s="1">
+      <c r="L10" s="14">
+        <v>0</v>
+      </c>
+      <c r="M10" s="1">
         <v>417</v>
       </c>
-      <c r="M10" s="1">
+      <c r="N10" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
         <v>115</v>
       </c>
@@ -1961,17 +1985,20 @@
       <c r="J11" s="2">
         <v>0</v>
       </c>
-      <c r="K11" s="15">
-        <v>0</v>
-      </c>
-      <c r="L11" s="2">
+      <c r="K11" s="2">
+        <v>0</v>
+      </c>
+      <c r="L11" s="15">
         <v>0</v>
       </c>
       <c r="M11" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>116</v>
       </c>
@@ -1997,22 +2024,25 @@
         <v>110</v>
       </c>
       <c r="I12" s="3">
+        <v>24</v>
+      </c>
+      <c r="J12" s="3">
         <v>760</v>
       </c>
-      <c r="J12" s="3">
+      <c r="K12" s="3">
         <v>473</v>
       </c>
-      <c r="K12" s="16">
+      <c r="L12" s="16">
         <v>378</v>
       </c>
-      <c r="L12" s="3">
+      <c r="M12" s="3">
         <v>420</v>
       </c>
-      <c r="M12" s="3">
+      <c r="N12" s="3">
         <v>459</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>117</v>
       </c>
@@ -2038,22 +2068,25 @@
         <v>204</v>
       </c>
       <c r="I13" s="3">
+        <v>189</v>
+      </c>
+      <c r="J13" s="3">
         <v>3004</v>
       </c>
-      <c r="J13" s="3">
+      <c r="K13" s="3">
         <v>1500</v>
       </c>
-      <c r="K13" s="16">
+      <c r="L13" s="16">
         <v>669</v>
       </c>
-      <c r="L13" s="3">
+      <c r="M13" s="3">
         <v>2056</v>
       </c>
-      <c r="M13" s="3">
+      <c r="N13" s="3">
         <v>1707</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>118</v>
       </c>
@@ -2079,22 +2112,25 @@
         <v>235</v>
       </c>
       <c r="I14" s="3">
+        <v>157</v>
+      </c>
+      <c r="J14" s="3">
         <v>5206</v>
       </c>
-      <c r="J14" s="3">
+      <c r="K14" s="3">
         <v>4216</v>
       </c>
-      <c r="K14" s="16">
+      <c r="L14" s="16">
         <v>627</v>
       </c>
-      <c r="L14" s="3">
+      <c r="M14" s="3">
         <v>3064</v>
       </c>
-      <c r="M14" s="3">
+      <c r="N14" s="3">
         <v>1338</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>119</v>
       </c>
@@ -2120,22 +2156,25 @@
         <v>215</v>
       </c>
       <c r="I15" s="3">
+        <v>50</v>
+      </c>
+      <c r="J15" s="3">
         <v>2725</v>
       </c>
-      <c r="J15" s="3">
+      <c r="K15" s="3">
         <v>2499</v>
       </c>
-      <c r="K15" s="16">
+      <c r="L15" s="16">
         <v>352</v>
       </c>
-      <c r="L15" s="3">
+      <c r="M15" s="3">
         <v>2229</v>
       </c>
-      <c r="M15" s="3">
+      <c r="N15" s="3">
         <v>980</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
         <v>120</v>
       </c>
@@ -2161,22 +2200,25 @@
         <v>13</v>
       </c>
       <c r="I16" s="2">
+        <v>0</v>
+      </c>
+      <c r="J16" s="2">
         <v>1575</v>
       </c>
-      <c r="J16" s="2">
+      <c r="K16" s="2">
         <v>1700</v>
       </c>
-      <c r="K16" s="15">
+      <c r="L16" s="15">
         <v>18</v>
       </c>
-      <c r="L16" s="2">
+      <c r="M16" s="2">
         <v>1478</v>
       </c>
-      <c r="M16" s="2">
+      <c r="N16" s="2">
         <v>322</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>121</v>
       </c>
@@ -2202,22 +2244,25 @@
         <v>67</v>
       </c>
       <c r="I17" s="1">
+        <v>0</v>
+      </c>
+      <c r="J17" s="1">
         <v>9370</v>
       </c>
-      <c r="J17" s="1">
+      <c r="K17" s="1">
         <v>17800</v>
       </c>
-      <c r="K17" s="14">
+      <c r="L17" s="14">
         <v>332</v>
       </c>
-      <c r="L17" s="1">
+      <c r="M17" s="1">
         <v>4517</v>
       </c>
-      <c r="M17" s="1">
+      <c r="N17" s="1">
         <v>5500</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
         <v>122</v>
       </c>
@@ -2243,22 +2288,25 @@
         <v>4</v>
       </c>
       <c r="I18" s="2">
+        <v>0</v>
+      </c>
+      <c r="J18" s="2">
         <v>1993</v>
       </c>
-      <c r="J18" s="2">
+      <c r="K18" s="2">
         <v>2720</v>
       </c>
-      <c r="K18" s="15">
+      <c r="L18" s="15">
         <v>8</v>
       </c>
-      <c r="L18" s="2">
+      <c r="M18" s="2">
         <v>1029</v>
       </c>
-      <c r="M18" s="2">
+      <c r="N18" s="2">
         <v>653</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>123</v>
       </c>
@@ -2284,22 +2332,25 @@
         <v>406</v>
       </c>
       <c r="I19" s="1">
+        <v>110</v>
+      </c>
+      <c r="J19" s="1">
         <v>15047</v>
       </c>
-      <c r="J19" s="1">
+      <c r="K19" s="1">
         <v>18840</v>
       </c>
-      <c r="K19" s="14">
+      <c r="L19" s="14">
         <v>330</v>
       </c>
-      <c r="L19" s="1">
+      <c r="M19" s="1">
         <v>3820</v>
       </c>
-      <c r="M19" s="1">
+      <c r="N19" s="1">
         <v>5168</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
         <v>124</v>
       </c>
@@ -2325,22 +2376,25 @@
         <v>667</v>
       </c>
       <c r="I20" s="2">
+        <v>0</v>
+      </c>
+      <c r="J20" s="2">
         <v>437</v>
       </c>
-      <c r="J20" s="2">
+      <c r="K20" s="2">
         <v>72</v>
       </c>
-      <c r="K20" s="15">
+      <c r="L20" s="15">
         <v>207</v>
       </c>
-      <c r="L20" s="2">
+      <c r="M20" s="2">
         <v>621</v>
       </c>
-      <c r="M20" s="2">
+      <c r="N20" s="2">
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>125</v>
       </c>
@@ -2366,22 +2420,25 @@
         <v>743</v>
       </c>
       <c r="I21" s="1">
+        <v>236</v>
+      </c>
+      <c r="J21" s="1">
         <v>16641</v>
       </c>
-      <c r="J21" s="1">
+      <c r="K21" s="1">
         <v>11614</v>
       </c>
-      <c r="K21" s="14">
+      <c r="L21" s="14">
         <v>553</v>
       </c>
-      <c r="L21" s="1">
+      <c r="M21" s="1">
         <v>3908</v>
       </c>
-      <c r="M21" s="1">
+      <c r="N21" s="1">
         <v>4861</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
         <v>126</v>
       </c>
@@ -2407,22 +2464,25 @@
         <v>506</v>
       </c>
       <c r="I22" s="2">
+        <v>17</v>
+      </c>
+      <c r="J22" s="2">
         <v>1331</v>
       </c>
-      <c r="J22" s="2">
+      <c r="K22" s="2">
         <v>545</v>
       </c>
-      <c r="K22" s="15">
+      <c r="L22" s="15">
         <v>99</v>
       </c>
-      <c r="L22" s="2">
+      <c r="M22" s="2">
         <v>822</v>
       </c>
-      <c r="M22" s="2">
+      <c r="N22" s="2">
         <v>308</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
         <v>127</v>
       </c>
@@ -2448,22 +2508,25 @@
         <v>594</v>
       </c>
       <c r="I23" s="1">
+        <v>0</v>
+      </c>
+      <c r="J23" s="1">
         <v>12421</v>
       </c>
-      <c r="J23" s="1">
+      <c r="K23" s="1">
         <v>16763</v>
       </c>
-      <c r="K23" s="14">
+      <c r="L23" s="14">
         <v>862</v>
       </c>
-      <c r="L23" s="1">
+      <c r="M23" s="1">
         <v>4189</v>
       </c>
-      <c r="M23" s="1">
+      <c r="N23" s="1">
         <v>6405</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
         <v>128</v>
       </c>
@@ -2489,22 +2552,25 @@
         <v>5749</v>
       </c>
       <c r="I24" s="2">
+        <v>0</v>
+      </c>
+      <c r="J24" s="2">
         <v>54804</v>
       </c>
-      <c r="J24" s="2">
+      <c r="K24" s="2">
         <v>57294</v>
       </c>
-      <c r="K24" s="15">
+      <c r="L24" s="15">
         <v>4500</v>
       </c>
-      <c r="L24" s="2">
+      <c r="M24" s="2">
         <v>12153</v>
       </c>
-      <c r="M24" s="2">
+      <c r="N24" s="2">
         <v>15572</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
         <v>129</v>
       </c>
@@ -2530,22 +2596,25 @@
         <v>313</v>
       </c>
       <c r="I25" s="1">
+        <v>0</v>
+      </c>
+      <c r="J25" s="1">
         <v>3636</v>
       </c>
-      <c r="J25" s="1">
+      <c r="K25" s="1">
         <v>4367</v>
       </c>
-      <c r="K25" s="14">
+      <c r="L25" s="14">
         <v>421</v>
       </c>
-      <c r="L25" s="1">
+      <c r="M25" s="1">
         <v>3319</v>
       </c>
-      <c r="M25" s="1">
+      <c r="N25" s="1">
         <v>1633</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="25" t="s">
         <v>130</v>
       </c>
@@ -2576,17 +2645,20 @@
       <c r="J26" s="2">
         <v>0</v>
       </c>
-      <c r="K26" s="15">
-        <v>0</v>
-      </c>
-      <c r="L26" s="2">
+      <c r="K26" s="2">
+        <v>0</v>
+      </c>
+      <c r="L26" s="15">
         <v>0</v>
       </c>
       <c r="M26" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N26" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
         <v>131</v>
       </c>
@@ -2612,22 +2684,25 @@
         <v>165</v>
       </c>
       <c r="I27" s="1">
+        <v>0</v>
+      </c>
+      <c r="J27" s="1">
         <v>5884</v>
       </c>
-      <c r="J27" s="1">
+      <c r="K27" s="1">
         <v>3509</v>
       </c>
-      <c r="K27" s="14">
+      <c r="L27" s="14">
         <v>183</v>
       </c>
-      <c r="L27" s="1">
+      <c r="M27" s="1">
         <v>1888</v>
       </c>
-      <c r="M27" s="1">
+      <c r="N27" s="1">
         <v>2078</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="25" t="s">
         <v>132</v>
       </c>
@@ -2653,22 +2728,25 @@
         <v>50</v>
       </c>
       <c r="I28" s="2">
+        <v>0</v>
+      </c>
+      <c r="J28" s="2">
         <v>1313</v>
       </c>
-      <c r="J28" s="2">
+      <c r="K28" s="2">
         <v>2254</v>
       </c>
-      <c r="K28" s="15">
+      <c r="L28" s="15">
         <v>15</v>
       </c>
-      <c r="L28" s="2">
+      <c r="M28" s="2">
         <v>745</v>
       </c>
-      <c r="M28" s="2">
+      <c r="N28" s="2">
         <v>487</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
         <v>133</v>
       </c>
@@ -2694,22 +2772,25 @@
         <v>95</v>
       </c>
       <c r="I29" s="1">
+        <v>324</v>
+      </c>
+      <c r="J29" s="1">
         <v>10626</v>
       </c>
-      <c r="J29" s="1">
+      <c r="K29" s="1">
         <v>15092</v>
       </c>
-      <c r="K29" s="14">
+      <c r="L29" s="14">
         <v>471</v>
       </c>
-      <c r="L29" s="1">
+      <c r="M29" s="1">
         <v>4446</v>
       </c>
-      <c r="M29" s="1">
+      <c r="N29" s="1">
         <v>4294</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="25" t="s">
         <v>134</v>
       </c>
@@ -2735,22 +2816,25 @@
         <v>360</v>
       </c>
       <c r="I30" s="2">
+        <v>0</v>
+      </c>
+      <c r="J30" s="2">
         <v>665</v>
       </c>
-      <c r="J30" s="2">
+      <c r="K30" s="2">
         <v>228</v>
       </c>
-      <c r="K30" s="15">
+      <c r="L30" s="15">
         <v>56</v>
       </c>
-      <c r="L30" s="2">
+      <c r="M30" s="2">
         <v>269</v>
       </c>
-      <c r="M30" s="2">
+      <c r="N30" s="2">
         <v>363</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
         <v>135</v>
       </c>
@@ -2776,22 +2860,25 @@
         <v>791</v>
       </c>
       <c r="I31" s="1">
+        <v>0</v>
+      </c>
+      <c r="J31" s="1">
         <v>1144</v>
       </c>
-      <c r="J31" s="1">
+      <c r="K31" s="1">
         <v>2586</v>
       </c>
-      <c r="K31" s="14">
+      <c r="L31" s="14">
         <v>271</v>
       </c>
-      <c r="L31" s="1">
+      <c r="M31" s="1">
         <v>2865</v>
       </c>
-      <c r="M31" s="1">
+      <c r="N31" s="1">
         <v>659</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="25" t="s">
         <v>136</v>
       </c>
@@ -2817,22 +2904,25 @@
         <v>858</v>
       </c>
       <c r="I32" s="2">
+        <v>0</v>
+      </c>
+      <c r="J32" s="2">
         <v>14821</v>
       </c>
-      <c r="J32" s="2">
+      <c r="K32" s="2">
         <v>7510</v>
       </c>
-      <c r="K32" s="15">
+      <c r="L32" s="15">
         <v>2728</v>
       </c>
-      <c r="L32" s="2">
+      <c r="M32" s="2">
         <v>5327</v>
       </c>
-      <c r="M32" s="2">
+      <c r="N32" s="2">
         <v>4625</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
         <v>137</v>
       </c>
@@ -2858,22 +2948,25 @@
         <v>148</v>
       </c>
       <c r="I33" s="1">
+        <v>1</v>
+      </c>
+      <c r="J33" s="1">
         <v>10216</v>
       </c>
-      <c r="J33" s="1">
+      <c r="K33" s="1">
         <v>7330</v>
       </c>
-      <c r="K33" s="14">
+      <c r="L33" s="14">
         <v>113</v>
       </c>
-      <c r="L33" s="1">
+      <c r="M33" s="1">
         <v>4895</v>
       </c>
-      <c r="M33" s="1">
+      <c r="N33" s="1">
         <v>3583</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="25" t="s">
         <v>138</v>
       </c>
@@ -2899,22 +2992,25 @@
         <v>167</v>
       </c>
       <c r="I34" s="2">
+        <v>0</v>
+      </c>
+      <c r="J34" s="2">
         <v>5192</v>
       </c>
-      <c r="J34" s="2">
+      <c r="K34" s="2">
         <v>3394</v>
       </c>
-      <c r="K34" s="15">
+      <c r="L34" s="15">
         <v>1984</v>
       </c>
-      <c r="L34" s="2">
+      <c r="M34" s="2">
         <v>1045</v>
       </c>
-      <c r="M34" s="2">
+      <c r="N34" s="2">
         <v>2107</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
         <v>139</v>
       </c>
@@ -2940,22 +3036,25 @@
         <v>2470</v>
       </c>
       <c r="I35" s="1">
+        <v>0</v>
+      </c>
+      <c r="J35" s="1">
         <v>36533</v>
       </c>
-      <c r="J35" s="1">
+      <c r="K35" s="1">
         <v>48158</v>
       </c>
-      <c r="K35" s="14">
+      <c r="L35" s="14">
         <v>2018</v>
       </c>
-      <c r="L35" s="1">
+      <c r="M35" s="1">
         <v>9239</v>
       </c>
-      <c r="M35" s="1">
+      <c r="N35" s="1">
         <v>9362</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="25" t="s">
         <v>140</v>
       </c>
@@ -2981,22 +3080,25 @@
         <v>729</v>
       </c>
       <c r="I36" s="2">
+        <v>0</v>
+      </c>
+      <c r="J36" s="2">
         <v>8094</v>
       </c>
-      <c r="J36" s="2">
+      <c r="K36" s="2">
         <v>5366</v>
       </c>
-      <c r="K36" s="15">
+      <c r="L36" s="15">
         <v>296</v>
       </c>
-      <c r="L36" s="2">
+      <c r="M36" s="2">
         <v>4526</v>
       </c>
-      <c r="M36" s="2">
+      <c r="N36" s="2">
         <v>1987</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
         <v>141</v>
       </c>
@@ -3022,22 +3124,25 @@
         <v>2029</v>
       </c>
       <c r="I37" s="1">
+        <v>511</v>
+      </c>
+      <c r="J37" s="1">
         <v>13514</v>
       </c>
-      <c r="J37" s="1">
+      <c r="K37" s="1">
         <v>16358</v>
       </c>
-      <c r="K37" s="14">
+      <c r="L37" s="14">
         <v>3809</v>
       </c>
-      <c r="L37" s="1">
+      <c r="M37" s="1">
         <v>3187</v>
       </c>
-      <c r="M37" s="1">
+      <c r="N37" s="1">
         <v>4566</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="25" t="s">
         <v>142</v>
       </c>
@@ -3063,22 +3168,25 @@
         <v>45</v>
       </c>
       <c r="I38" s="2">
+        <v>0</v>
+      </c>
+      <c r="J38" s="2">
         <v>717</v>
       </c>
-      <c r="J38" s="2">
+      <c r="K38" s="2">
         <v>848</v>
       </c>
-      <c r="K38" s="15">
+      <c r="L38" s="15">
         <v>7</v>
       </c>
-      <c r="L38" s="2">
+      <c r="M38" s="2">
         <v>1512</v>
       </c>
-      <c r="M38" s="2">
+      <c r="N38" s="2">
         <v>270</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
         <v>143</v>
       </c>
@@ -3104,22 +3212,25 @@
         <v>69</v>
       </c>
       <c r="I39" s="1">
+        <v>0</v>
+      </c>
+      <c r="J39" s="1">
         <v>578</v>
       </c>
-      <c r="J39" s="1">
+      <c r="K39" s="1">
         <v>2123</v>
       </c>
-      <c r="K39" s="14">
+      <c r="L39" s="14">
         <v>60</v>
       </c>
-      <c r="L39" s="1">
+      <c r="M39" s="1">
         <v>776</v>
       </c>
-      <c r="M39" s="1">
+      <c r="N39" s="1">
         <v>1105</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="18" t="s">
         <v>144</v>
       </c>
@@ -3145,22 +3256,25 @@
         <v>105</v>
       </c>
       <c r="I40" s="5">
+        <v>0</v>
+      </c>
+      <c r="J40" s="5">
         <v>108</v>
       </c>
-      <c r="J40" s="5">
+      <c r="K40" s="5">
         <v>3921</v>
       </c>
-      <c r="K40" s="18">
+      <c r="L40" s="18">
         <v>73</v>
       </c>
-      <c r="L40" s="5">
+      <c r="M40" s="5">
         <v>602</v>
       </c>
-      <c r="M40" s="5">
+      <c r="N40" s="5">
         <v>181</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="18" t="s">
         <v>145</v>
       </c>
@@ -3186,22 +3300,25 @@
         <v>242</v>
       </c>
       <c r="I41" s="5">
+        <v>0</v>
+      </c>
+      <c r="J41" s="5">
         <v>76</v>
       </c>
-      <c r="J41" s="5">
+      <c r="K41" s="5">
         <v>16624</v>
       </c>
-      <c r="K41" s="18">
+      <c r="L41" s="18">
         <v>63</v>
       </c>
-      <c r="L41" s="5">
+      <c r="M41" s="5">
         <v>935</v>
       </c>
-      <c r="M41" s="5">
+      <c r="N41" s="5">
         <v>555</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="18" t="s">
         <v>146</v>
       </c>
@@ -3227,22 +3344,25 @@
         <v>97</v>
       </c>
       <c r="I42" s="5">
+        <v>0</v>
+      </c>
+      <c r="J42" s="5">
         <v>346</v>
       </c>
-      <c r="J42" s="5">
+      <c r="K42" s="5">
         <v>51</v>
       </c>
-      <c r="K42" s="18">
+      <c r="L42" s="18">
         <v>13</v>
       </c>
-      <c r="L42" s="5">
+      <c r="M42" s="5">
         <v>190</v>
       </c>
-      <c r="M42" s="5">
+      <c r="N42" s="5">
         <v>79</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="18" t="s">
         <v>147</v>
       </c>
@@ -3268,22 +3388,25 @@
         <v>118</v>
       </c>
       <c r="I43" s="5">
+        <v>0</v>
+      </c>
+      <c r="J43" s="5">
         <v>13</v>
       </c>
-      <c r="J43" s="5">
+      <c r="K43" s="5">
         <v>1428</v>
       </c>
-      <c r="K43" s="18">
-        <v>0</v>
-      </c>
-      <c r="L43" s="5">
+      <c r="L43" s="18">
+        <v>0</v>
+      </c>
+      <c r="M43" s="5">
         <v>152</v>
       </c>
-      <c r="M43" s="5">
+      <c r="N43" s="5">
         <v>134</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="18" t="s">
         <v>148</v>
       </c>
@@ -3309,22 +3432,25 @@
         <v>210</v>
       </c>
       <c r="I44" s="5">
+        <v>0</v>
+      </c>
+      <c r="J44" s="5">
         <v>643</v>
       </c>
-      <c r="J44" s="5">
+      <c r="K44" s="5">
         <v>2744</v>
       </c>
-      <c r="K44" s="18">
+      <c r="L44" s="18">
         <v>27</v>
       </c>
-      <c r="L44" s="5">
+      <c r="M44" s="5">
         <v>14</v>
       </c>
-      <c r="M44" s="5">
+      <c r="N44" s="5">
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
         <v>149</v>
       </c>
@@ -3350,22 +3476,25 @@
         <v>66</v>
       </c>
       <c r="I45" s="1">
+        <v>0</v>
+      </c>
+      <c r="J45" s="1">
         <v>1793</v>
       </c>
-      <c r="J45" s="1">
+      <c r="K45" s="1">
         <v>1747</v>
       </c>
-      <c r="K45" s="14">
+      <c r="L45" s="14">
         <v>1781</v>
       </c>
-      <c r="L45" s="1">
+      <c r="M45" s="1">
         <v>1527</v>
       </c>
-      <c r="M45" s="1">
+      <c r="N45" s="1">
         <v>739</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="25" t="s">
         <v>150</v>
       </c>
@@ -3391,22 +3520,25 @@
         <v>83</v>
       </c>
       <c r="I46" s="2">
+        <v>0</v>
+      </c>
+      <c r="J46" s="2">
         <v>10107</v>
       </c>
-      <c r="J46" s="2">
+      <c r="K46" s="2">
         <v>9883</v>
       </c>
-      <c r="K46" s="15">
+      <c r="L46" s="15">
         <v>478</v>
       </c>
-      <c r="L46" s="2">
+      <c r="M46" s="2">
         <v>5840</v>
       </c>
-      <c r="M46" s="2">
+      <c r="N46" s="2">
         <v>3647</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
         <v>151</v>
       </c>
@@ -3432,22 +3564,25 @@
         <v>668</v>
       </c>
       <c r="I47" s="1">
+        <v>587</v>
+      </c>
+      <c r="J47" s="1">
         <v>12891</v>
       </c>
-      <c r="J47" s="1">
+      <c r="K47" s="1">
         <v>35108</v>
       </c>
-      <c r="K47" s="14">
+      <c r="L47" s="14">
         <v>1217</v>
       </c>
-      <c r="L47" s="1">
+      <c r="M47" s="1">
         <v>5711</v>
       </c>
-      <c r="M47" s="1">
+      <c r="N47" s="1">
         <v>7191</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="25" t="s">
         <v>152</v>
       </c>
@@ -3473,22 +3608,25 @@
         <v>17</v>
       </c>
       <c r="I48" s="2">
+        <v>58</v>
+      </c>
+      <c r="J48" s="2">
         <v>9122</v>
       </c>
-      <c r="J48" s="2">
+      <c r="K48" s="2">
         <v>14136</v>
       </c>
-      <c r="K48" s="15">
+      <c r="L48" s="15">
         <v>37</v>
       </c>
-      <c r="L48" s="2">
+      <c r="M48" s="2">
         <v>5707</v>
       </c>
-      <c r="M48" s="2">
+      <c r="N48" s="2">
         <v>2134</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
         <v>153</v>
       </c>
@@ -3514,22 +3652,25 @@
         <v>943</v>
       </c>
       <c r="I49" s="1">
+        <v>162</v>
+      </c>
+      <c r="J49" s="1">
         <v>5785</v>
       </c>
-      <c r="J49" s="1">
+      <c r="K49" s="1">
         <v>11235</v>
       </c>
-      <c r="K49" s="14">
+      <c r="L49" s="14">
         <v>988</v>
       </c>
-      <c r="L49" s="1">
+      <c r="M49" s="1">
         <v>2116</v>
       </c>
-      <c r="M49" s="1">
+      <c r="N49" s="1">
         <v>3051</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="25" t="s">
         <v>154</v>
       </c>
@@ -3555,22 +3696,25 @@
         <v>624</v>
       </c>
       <c r="I50" s="2">
+        <v>0</v>
+      </c>
+      <c r="J50" s="2">
         <v>18075</v>
       </c>
-      <c r="J50" s="2">
+      <c r="K50" s="2">
         <v>24148</v>
       </c>
-      <c r="K50" s="15">
+      <c r="L50" s="15">
         <v>3986</v>
       </c>
-      <c r="L50" s="2">
+      <c r="M50" s="2">
         <v>4890</v>
       </c>
-      <c r="M50" s="2">
+      <c r="N50" s="2">
         <v>8046</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
         <v>155</v>
       </c>
@@ -3596,22 +3740,25 @@
         <v>66</v>
       </c>
       <c r="I51" s="1">
+        <v>0</v>
+      </c>
+      <c r="J51" s="1">
         <v>3843</v>
       </c>
-      <c r="J51" s="1">
+      <c r="K51" s="1">
         <v>2728</v>
       </c>
-      <c r="K51" s="14">
+      <c r="L51" s="14">
         <v>21</v>
       </c>
-      <c r="L51" s="1">
+      <c r="M51" s="1">
         <v>1229</v>
       </c>
-      <c r="M51" s="1">
+      <c r="N51" s="1">
         <v>1930</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="25" t="s">
         <v>156</v>
       </c>
@@ -3637,22 +3784,25 @@
         <v>736</v>
       </c>
       <c r="I52" s="2">
+        <v>0</v>
+      </c>
+      <c r="J52" s="2">
         <v>8370</v>
       </c>
-      <c r="J52" s="2">
+      <c r="K52" s="2">
         <v>13427</v>
       </c>
-      <c r="K52" s="15">
+      <c r="L52" s="15">
         <v>1221</v>
       </c>
-      <c r="L52" s="2">
+      <c r="M52" s="2">
         <v>4751</v>
       </c>
-      <c r="M52" s="2">
+      <c r="N52" s="2">
         <v>3971</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
         <v>157</v>
       </c>
@@ -3678,22 +3828,25 @@
         <v>169</v>
       </c>
       <c r="I53" s="1">
+        <v>0</v>
+      </c>
+      <c r="J53" s="1">
         <v>2510</v>
       </c>
-      <c r="J53" s="1">
+      <c r="K53" s="1">
         <v>1041</v>
       </c>
-      <c r="K53" s="14">
+      <c r="L53" s="14">
         <v>74</v>
       </c>
-      <c r="L53" s="1">
+      <c r="M53" s="1">
         <v>2218</v>
       </c>
-      <c r="M53" s="1">
+      <c r="N53" s="1">
         <v>1238</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="25" t="s">
         <v>158</v>
       </c>
@@ -3719,22 +3872,25 @@
         <v>42</v>
       </c>
       <c r="I54" s="2">
+        <v>0</v>
+      </c>
+      <c r="J54" s="2">
         <v>1222</v>
       </c>
-      <c r="J54" s="2">
+      <c r="K54" s="2">
         <v>2162</v>
       </c>
-      <c r="K54" s="15">
+      <c r="L54" s="15">
         <v>17</v>
       </c>
-      <c r="L54" s="2">
+      <c r="M54" s="2">
         <v>2066</v>
       </c>
-      <c r="M54" s="2">
+      <c r="N54" s="2">
         <v>225</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
         <v>159</v>
       </c>
@@ -3760,22 +3916,25 @@
         <v>11</v>
       </c>
       <c r="I55" s="1">
+        <v>0</v>
+      </c>
+      <c r="J55" s="1">
         <v>2786</v>
       </c>
-      <c r="J55" s="1">
+      <c r="K55" s="1">
         <v>2439</v>
       </c>
-      <c r="K55" s="14">
+      <c r="L55" s="14">
         <v>9</v>
       </c>
-      <c r="L55" s="1">
+      <c r="M55" s="1">
         <v>1765</v>
       </c>
-      <c r="M55" s="1">
+      <c r="N55" s="1">
         <v>2308</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="20" t="s">
         <v>160</v>
       </c>
@@ -3784,7 +3943,7 @@
         <v>2381</v>
       </c>
       <c r="C56" s="20">
-        <f t="shared" ref="C56:M56" si="0">SUM(C12:C15)</f>
+        <f t="shared" ref="C56:N56" si="0">SUM(C12:C15)</f>
         <v>19374</v>
       </c>
       <c r="D56" s="20">
@@ -3808,27 +3967,31 @@
         <v>764</v>
       </c>
       <c r="I56" s="20">
+        <f t="shared" ref="I56" si="1">SUM(I12:I15)</f>
+        <v>420</v>
+      </c>
+      <c r="J56" s="20">
         <f t="shared" si="0"/>
         <v>11695</v>
       </c>
-      <c r="J56" s="20">
+      <c r="K56" s="20">
         <f t="shared" si="0"/>
         <v>8688</v>
       </c>
-      <c r="K56" s="20">
+      <c r="L56" s="20">
         <f t="shared" si="0"/>
         <v>2026</v>
       </c>
-      <c r="L56" s="20">
+      <c r="M56" s="20">
         <f t="shared" si="0"/>
         <v>7769</v>
       </c>
-      <c r="M56" s="20">
+      <c r="N56" s="20">
         <f t="shared" si="0"/>
         <v>4484</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="22" t="s">
         <v>161</v>
       </c>
@@ -3837,51 +4000,55 @@
         <v>1422</v>
       </c>
       <c r="C57" s="22">
-        <f t="shared" ref="C57:M57" si="1">SUM(C40:C44)</f>
+        <f t="shared" ref="C57:N57" si="2">SUM(C40:C44)</f>
         <v>49765</v>
       </c>
       <c r="D57" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>207</v>
       </c>
       <c r="E57" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>958</v>
       </c>
       <c r="F57" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>74</v>
       </c>
       <c r="G57" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>108</v>
       </c>
       <c r="H57" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>772</v>
       </c>
       <c r="I57" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="I57" si="3">SUM(I40:I44)</f>
+        <v>0</v>
+      </c>
+      <c r="J57" s="22">
+        <f t="shared" si="2"/>
         <v>1186</v>
       </c>
-      <c r="J57" s="22">
-        <f t="shared" si="1"/>
+      <c r="K57" s="22">
+        <f t="shared" si="2"/>
         <v>24768</v>
       </c>
-      <c r="K57" s="22">
-        <f t="shared" si="1"/>
+      <c r="L57" s="22">
+        <f t="shared" si="2"/>
         <v>176</v>
       </c>
-      <c r="L57" s="22">
-        <f t="shared" si="1"/>
+      <c r="M57" s="22">
+        <f t="shared" si="2"/>
         <v>1893</v>
       </c>
-      <c r="M57" s="22">
-        <f t="shared" si="1"/>
+      <c r="N57" s="22">
+        <f t="shared" si="2"/>
         <v>956</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="21" t="s">
         <v>162</v>
       </c>
@@ -3890,59 +4057,63 @@
         <v>116529</v>
       </c>
       <c r="C58" s="21">
-        <f t="shared" ref="C58:M58" si="2">SUM(C2:C55)</f>
+        <f t="shared" ref="C58:N58" si="4">SUM(C2:C55)</f>
         <v>822910</v>
       </c>
       <c r="D58" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>27388</v>
       </c>
       <c r="E58" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>57085</v>
       </c>
       <c r="F58" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>34840</v>
       </c>
       <c r="G58" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>115890</v>
       </c>
       <c r="H58" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>27390</v>
       </c>
       <c r="I58" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="I58" si="5">SUM(I2:I55)</f>
+        <v>2750</v>
+      </c>
+      <c r="J58" s="21">
+        <f t="shared" si="4"/>
         <v>457234</v>
       </c>
-      <c r="J58" s="21">
-        <f t="shared" si="2"/>
+      <c r="K58" s="21">
+        <f t="shared" si="4"/>
         <v>573667</v>
       </c>
-      <c r="K58" s="21">
-        <f t="shared" si="2"/>
+      <c r="L58" s="21">
+        <f t="shared" si="4"/>
         <v>42383</v>
       </c>
-      <c r="L58" s="21">
-        <f t="shared" si="2"/>
+      <c r="M58" s="21">
+        <f t="shared" si="4"/>
         <v>170301</v>
       </c>
-      <c r="M58" s="21">
-        <f t="shared" si="2"/>
+      <c r="N58" s="21">
+        <f t="shared" si="4"/>
         <v>157081</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="25"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M58" xr:uid="{D90AFE98-8C78-4B1F-BEC8-FD4085F25E61}"/>
+  <autoFilter ref="A1:N58" xr:uid="{D90AFE98-8C78-4B1F-BEC8-FD4085F25E61}"/>
   <dataValidations count="3">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Based on the monthly circulation spreadsheet as run on January 1, 2024 and throughout 2023" sqref="B1 L1:M1" xr:uid="{4F697491-ED7E-4CD5-8B7B-C8361B45F1C6}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Data from Item count by item type spreadsheet" sqref="C1:H1" xr:uid="{EBA39581-4BBC-422D-808C-F87F8349E2FC}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Based on circulation by item type spreadsheet as run on January 1, 2024 and throughout 2023" sqref="I1:K1" xr:uid="{B84C8F23-D037-4B3C-BA10-CDDBCB4699DA}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Based on the monthly circulation spreadsheet as run on January 1, 2024 and throughout 2023" sqref="B1 M1:N1" xr:uid="{4F697491-ED7E-4CD5-8B7B-C8361B45F1C6}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Data from Item count by item type spreadsheet" sqref="C1:I1" xr:uid="{EBA39581-4BBC-422D-808C-F87F8349E2FC}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Based on circulation by item type spreadsheet as run on January 1, 2024 and throughout 2023" sqref="J1:L1" xr:uid="{B84C8F23-D037-4B3C-BA10-CDDBCB4699DA}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update to fix error
</commit_message>
<xml_diff>
--- a/statistics_files/2023/99.year.end/2023.state.survey.xlsx
+++ b/statistics_files/2023/99.year.end/2023.state.survey.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\GitHub\next_statistics\statistics_files\2023\99.year.end\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EDBF630-AE39-457D-AAFA-2085F6BADEAA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A512976C-FDCB-4D94-920F-D93A37641B52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11295" tabRatio="717" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1587,16 +1587,16 @@
         <v>0</v>
       </c>
       <c r="J2" s="1">
-        <v>34429</v>
+        <v>31665</v>
       </c>
       <c r="K2" s="1">
-        <v>37031</v>
+        <v>38004</v>
       </c>
       <c r="L2" s="14">
-        <v>1462</v>
+        <v>652</v>
       </c>
       <c r="M2" s="1">
-        <v>11009</v>
+        <v>870</v>
       </c>
       <c r="N2" s="1">
         <v>12393</v>
@@ -1631,16 +1631,16 @@
         <v>60</v>
       </c>
       <c r="J3" s="2">
-        <v>15036</v>
+        <v>15950</v>
       </c>
       <c r="K3" s="2">
-        <v>18825</v>
+        <v>21772</v>
       </c>
       <c r="L3" s="15">
-        <v>1127</v>
+        <v>513</v>
       </c>
       <c r="M3" s="2">
-        <v>4354</v>
+        <v>116</v>
       </c>
       <c r="N3" s="2">
         <v>4376</v>
@@ -1675,16 +1675,16 @@
         <v>34</v>
       </c>
       <c r="J4" s="1">
-        <v>48424</v>
+        <v>44678</v>
       </c>
       <c r="K4" s="1">
-        <v>70073</v>
+        <v>73561</v>
       </c>
       <c r="L4" s="14">
-        <v>3814</v>
+        <v>2918</v>
       </c>
       <c r="M4" s="1">
-        <v>11464</v>
+        <v>297</v>
       </c>
       <c r="N4" s="1">
         <v>10633</v>
@@ -1719,16 +1719,16 @@
         <v>0</v>
       </c>
       <c r="J5" s="2">
-        <v>1176</v>
+        <v>1340</v>
       </c>
       <c r="K5" s="2">
-        <v>1263</v>
+        <v>1392</v>
       </c>
       <c r="L5" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M5" s="2">
-        <v>1098</v>
+        <v>14</v>
       </c>
       <c r="N5" s="2">
         <v>267</v>
@@ -1763,16 +1763,16 @@
         <v>59</v>
       </c>
       <c r="J6" s="1">
-        <v>29178</v>
+        <v>32919</v>
       </c>
       <c r="K6" s="1">
-        <v>40691</v>
+        <v>44048</v>
       </c>
       <c r="L6" s="14">
-        <v>3201</v>
+        <v>1013</v>
       </c>
       <c r="M6" s="1">
-        <v>13217</v>
+        <v>683</v>
       </c>
       <c r="N6" s="1">
         <v>10303</v>
@@ -1807,16 +1807,16 @@
         <v>171</v>
       </c>
       <c r="J7" s="2">
-        <v>4785</v>
+        <v>4080</v>
       </c>
       <c r="K7" s="2">
-        <v>2891</v>
+        <v>3597</v>
       </c>
       <c r="L7" s="15">
-        <v>1334</v>
+        <v>529</v>
       </c>
       <c r="M7" s="2">
-        <v>2168</v>
+        <v>29</v>
       </c>
       <c r="N7" s="2">
         <v>1753</v>
@@ -1851,16 +1851,16 @@
         <v>0</v>
       </c>
       <c r="J8" s="1">
-        <v>5938</v>
+        <v>5872</v>
       </c>
       <c r="K8" s="1">
-        <v>3310</v>
+        <v>3500</v>
       </c>
       <c r="L8" s="14">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="M8" s="1">
-        <v>1832</v>
+        <v>0</v>
       </c>
       <c r="N8" s="1">
         <v>1016</v>
@@ -1895,16 +1895,16 @@
         <v>0</v>
       </c>
       <c r="J9" s="2">
-        <v>2189</v>
+        <v>2651</v>
       </c>
       <c r="K9" s="2">
-        <v>1271</v>
+        <v>1866</v>
       </c>
       <c r="L9" s="15">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="M9" s="2">
-        <v>684</v>
+        <v>0</v>
       </c>
       <c r="N9" s="2">
         <v>445</v>
@@ -1939,16 +1939,16 @@
         <v>0</v>
       </c>
       <c r="J10" s="1">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="K10" s="1">
-        <v>331</v>
+        <v>310</v>
       </c>
       <c r="L10" s="14">
         <v>0</v>
       </c>
       <c r="M10" s="1">
-        <v>417</v>
+        <v>0</v>
       </c>
       <c r="N10" s="1">
         <v>32</v>
@@ -1983,10 +1983,10 @@
         <v>0</v>
       </c>
       <c r="J11" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L11" s="15">
         <v>0</v>
@@ -2027,16 +2027,16 @@
         <v>24</v>
       </c>
       <c r="J12" s="3">
-        <v>760</v>
+        <v>790</v>
       </c>
       <c r="K12" s="3">
-        <v>473</v>
+        <v>575</v>
       </c>
       <c r="L12" s="16">
-        <v>378</v>
+        <v>71</v>
       </c>
       <c r="M12" s="3">
-        <v>420</v>
+        <v>244</v>
       </c>
       <c r="N12" s="3">
         <v>459</v>
@@ -2071,16 +2071,16 @@
         <v>189</v>
       </c>
       <c r="J13" s="3">
-        <v>3004</v>
+        <v>2985</v>
       </c>
       <c r="K13" s="3">
-        <v>1500</v>
+        <v>1679</v>
       </c>
       <c r="L13" s="16">
-        <v>669</v>
+        <v>272</v>
       </c>
       <c r="M13" s="3">
-        <v>2056</v>
+        <v>195</v>
       </c>
       <c r="N13" s="3">
         <v>1707</v>
@@ -2115,16 +2115,16 @@
         <v>157</v>
       </c>
       <c r="J14" s="3">
-        <v>5206</v>
+        <v>4439</v>
       </c>
       <c r="K14" s="3">
-        <v>4216</v>
+        <v>3365</v>
       </c>
       <c r="L14" s="16">
-        <v>627</v>
+        <v>338</v>
       </c>
       <c r="M14" s="3">
-        <v>3064</v>
+        <v>43</v>
       </c>
       <c r="N14" s="3">
         <v>1338</v>
@@ -2159,16 +2159,16 @@
         <v>50</v>
       </c>
       <c r="J15" s="3">
-        <v>2725</v>
+        <v>2764</v>
       </c>
       <c r="K15" s="3">
-        <v>2499</v>
+        <v>2931</v>
       </c>
       <c r="L15" s="16">
-        <v>352</v>
+        <v>154</v>
       </c>
       <c r="M15" s="3">
-        <v>2229</v>
+        <v>34</v>
       </c>
       <c r="N15" s="3">
         <v>980</v>
@@ -2203,16 +2203,16 @@
         <v>0</v>
       </c>
       <c r="J16" s="2">
-        <v>1575</v>
+        <v>1556</v>
       </c>
       <c r="K16" s="2">
-        <v>1700</v>
+        <v>1950</v>
       </c>
       <c r="L16" s="15">
-        <v>18</v>
+        <v>65</v>
       </c>
       <c r="M16" s="2">
-        <v>1478</v>
+        <v>0</v>
       </c>
       <c r="N16" s="2">
         <v>322</v>
@@ -2247,16 +2247,16 @@
         <v>0</v>
       </c>
       <c r="J17" s="1">
-        <v>9370</v>
+        <v>10200</v>
       </c>
       <c r="K17" s="1">
-        <v>17800</v>
+        <v>17902</v>
       </c>
       <c r="L17" s="14">
-        <v>332</v>
+        <v>141</v>
       </c>
       <c r="M17" s="1">
-        <v>4517</v>
+        <v>144</v>
       </c>
       <c r="N17" s="1">
         <v>5500</v>
@@ -2291,16 +2291,16 @@
         <v>0</v>
       </c>
       <c r="J18" s="2">
-        <v>1993</v>
+        <v>721</v>
       </c>
       <c r="K18" s="2">
-        <v>2720</v>
+        <v>1704</v>
       </c>
       <c r="L18" s="15">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="M18" s="2">
-        <v>1029</v>
+        <v>0</v>
       </c>
       <c r="N18" s="2">
         <v>653</v>
@@ -2335,16 +2335,16 @@
         <v>110</v>
       </c>
       <c r="J19" s="1">
-        <v>15047</v>
+        <v>13766</v>
       </c>
       <c r="K19" s="1">
-        <v>18840</v>
+        <v>16100</v>
       </c>
       <c r="L19" s="14">
-        <v>330</v>
+        <v>188</v>
       </c>
       <c r="M19" s="1">
-        <v>3820</v>
+        <v>0</v>
       </c>
       <c r="N19" s="1">
         <v>5168</v>
@@ -2379,16 +2379,16 @@
         <v>0</v>
       </c>
       <c r="J20" s="2">
-        <v>437</v>
+        <v>339</v>
       </c>
       <c r="K20" s="2">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="L20" s="15">
-        <v>207</v>
+        <v>95</v>
       </c>
       <c r="M20" s="2">
-        <v>621</v>
+        <v>0</v>
       </c>
       <c r="N20" s="2">
         <v>35</v>
@@ -2423,16 +2423,16 @@
         <v>236</v>
       </c>
       <c r="J21" s="1">
-        <v>16641</v>
+        <v>16184</v>
       </c>
       <c r="K21" s="1">
-        <v>11614</v>
+        <v>11360</v>
       </c>
       <c r="L21" s="14">
-        <v>553</v>
+        <v>419</v>
       </c>
       <c r="M21" s="1">
-        <v>3908</v>
+        <v>0</v>
       </c>
       <c r="N21" s="1">
         <v>4861</v>
@@ -2467,16 +2467,16 @@
         <v>17</v>
       </c>
       <c r="J22" s="2">
-        <v>1331</v>
+        <v>1363</v>
       </c>
       <c r="K22" s="2">
-        <v>545</v>
+        <v>461</v>
       </c>
       <c r="L22" s="15">
-        <v>99</v>
+        <v>30</v>
       </c>
       <c r="M22" s="2">
-        <v>822</v>
+        <v>0</v>
       </c>
       <c r="N22" s="2">
         <v>308</v>
@@ -2511,16 +2511,16 @@
         <v>0</v>
       </c>
       <c r="J23" s="1">
-        <v>12421</v>
+        <v>13504</v>
       </c>
       <c r="K23" s="1">
-        <v>16763</v>
+        <v>18309</v>
       </c>
       <c r="L23" s="14">
-        <v>862</v>
+        <v>842</v>
       </c>
       <c r="M23" s="1">
-        <v>4189</v>
+        <v>19</v>
       </c>
       <c r="N23" s="1">
         <v>6405</v>
@@ -2555,16 +2555,16 @@
         <v>0</v>
       </c>
       <c r="J24" s="2">
-        <v>54804</v>
+        <v>59749</v>
       </c>
       <c r="K24" s="2">
-        <v>57294</v>
+        <v>65286</v>
       </c>
       <c r="L24" s="15">
-        <v>4500</v>
+        <v>2910</v>
       </c>
       <c r="M24" s="2">
-        <v>12153</v>
+        <v>676</v>
       </c>
       <c r="N24" s="2">
         <v>15572</v>
@@ -2599,16 +2599,16 @@
         <v>0</v>
       </c>
       <c r="J25" s="1">
-        <v>3636</v>
+        <v>3697</v>
       </c>
       <c r="K25" s="1">
-        <v>4367</v>
+        <v>5871</v>
       </c>
       <c r="L25" s="14">
-        <v>421</v>
+        <v>477</v>
       </c>
       <c r="M25" s="1">
-        <v>3319</v>
+        <v>0</v>
       </c>
       <c r="N25" s="1">
         <v>1633</v>
@@ -2687,16 +2687,16 @@
         <v>0</v>
       </c>
       <c r="J27" s="1">
-        <v>5884</v>
+        <v>5199</v>
       </c>
       <c r="K27" s="1">
-        <v>3509</v>
+        <v>3137</v>
       </c>
       <c r="L27" s="14">
-        <v>183</v>
+        <v>385</v>
       </c>
       <c r="M27" s="1">
-        <v>1888</v>
+        <v>1</v>
       </c>
       <c r="N27" s="1">
         <v>2078</v>
@@ -2731,16 +2731,16 @@
         <v>0</v>
       </c>
       <c r="J28" s="2">
-        <v>1313</v>
+        <v>943</v>
       </c>
       <c r="K28" s="2">
-        <v>2254</v>
+        <v>1361</v>
       </c>
       <c r="L28" s="15">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="M28" s="2">
-        <v>745</v>
+        <v>0</v>
       </c>
       <c r="N28" s="2">
         <v>487</v>
@@ -2775,16 +2775,16 @@
         <v>324</v>
       </c>
       <c r="J29" s="1">
-        <v>10626</v>
+        <v>9306</v>
       </c>
       <c r="K29" s="1">
-        <v>15092</v>
+        <v>14164</v>
       </c>
       <c r="L29" s="14">
-        <v>471</v>
+        <v>420</v>
       </c>
       <c r="M29" s="1">
-        <v>4446</v>
+        <v>0</v>
       </c>
       <c r="N29" s="1">
         <v>4294</v>
@@ -2819,16 +2819,16 @@
         <v>0</v>
       </c>
       <c r="J30" s="2">
-        <v>665</v>
+        <v>483</v>
       </c>
       <c r="K30" s="2">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="L30" s="15">
-        <v>56</v>
+        <v>18</v>
       </c>
       <c r="M30" s="2">
-        <v>269</v>
+        <v>16</v>
       </c>
       <c r="N30" s="2">
         <v>363</v>
@@ -2863,16 +2863,16 @@
         <v>0</v>
       </c>
       <c r="J31" s="1">
-        <v>1144</v>
+        <v>1592</v>
       </c>
       <c r="K31" s="1">
-        <v>2586</v>
+        <v>2628</v>
       </c>
       <c r="L31" s="14">
-        <v>271</v>
+        <v>201</v>
       </c>
       <c r="M31" s="1">
-        <v>2865</v>
+        <v>0</v>
       </c>
       <c r="N31" s="1">
         <v>659</v>
@@ -2907,16 +2907,16 @@
         <v>0</v>
       </c>
       <c r="J32" s="2">
-        <v>14821</v>
+        <v>14772</v>
       </c>
       <c r="K32" s="2">
-        <v>7510</v>
+        <v>8492</v>
       </c>
       <c r="L32" s="15">
-        <v>2728</v>
+        <v>2751</v>
       </c>
       <c r="M32" s="2">
-        <v>5327</v>
+        <v>306</v>
       </c>
       <c r="N32" s="2">
         <v>4625</v>
@@ -2951,16 +2951,16 @@
         <v>1</v>
       </c>
       <c r="J33" s="1">
-        <v>10216</v>
+        <v>8931</v>
       </c>
       <c r="K33" s="1">
-        <v>7330</v>
+        <v>7673</v>
       </c>
       <c r="L33" s="14">
-        <v>113</v>
+        <v>129</v>
       </c>
       <c r="M33" s="1">
-        <v>4895</v>
+        <v>0</v>
       </c>
       <c r="N33" s="1">
         <v>3583</v>
@@ -2995,16 +2995,16 @@
         <v>0</v>
       </c>
       <c r="J34" s="2">
-        <v>5192</v>
+        <v>4508</v>
       </c>
       <c r="K34" s="2">
-        <v>3394</v>
+        <v>3164</v>
       </c>
       <c r="L34" s="15">
-        <v>1984</v>
+        <v>1573</v>
       </c>
       <c r="M34" s="2">
-        <v>1045</v>
+        <v>0</v>
       </c>
       <c r="N34" s="2">
         <v>2107</v>
@@ -3039,16 +3039,16 @@
         <v>0</v>
       </c>
       <c r="J35" s="1">
-        <v>36533</v>
+        <v>36080</v>
       </c>
       <c r="K35" s="1">
-        <v>48158</v>
+        <v>54815</v>
       </c>
       <c r="L35" s="14">
-        <v>2018</v>
+        <v>1753</v>
       </c>
       <c r="M35" s="1">
-        <v>9239</v>
+        <v>219</v>
       </c>
       <c r="N35" s="1">
         <v>9362</v>
@@ -3083,16 +3083,16 @@
         <v>0</v>
       </c>
       <c r="J36" s="2">
-        <v>8094</v>
+        <v>8100</v>
       </c>
       <c r="K36" s="2">
-        <v>5366</v>
+        <v>5435</v>
       </c>
       <c r="L36" s="15">
-        <v>296</v>
+        <v>186</v>
       </c>
       <c r="M36" s="2">
-        <v>4526</v>
+        <v>77</v>
       </c>
       <c r="N36" s="2">
         <v>1987</v>
@@ -3127,16 +3127,16 @@
         <v>511</v>
       </c>
       <c r="J37" s="1">
-        <v>13514</v>
+        <v>14659</v>
       </c>
       <c r="K37" s="1">
-        <v>16358</v>
+        <v>22937</v>
       </c>
       <c r="L37" s="14">
-        <v>3809</v>
+        <v>4579</v>
       </c>
       <c r="M37" s="1">
-        <v>3187</v>
+        <v>0</v>
       </c>
       <c r="N37" s="1">
         <v>4566</v>
@@ -3171,16 +3171,16 @@
         <v>0</v>
       </c>
       <c r="J38" s="2">
-        <v>717</v>
+        <v>569</v>
       </c>
       <c r="K38" s="2">
-        <v>848</v>
+        <v>991</v>
       </c>
       <c r="L38" s="15">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="M38" s="2">
-        <v>1512</v>
+        <v>4</v>
       </c>
       <c r="N38" s="2">
         <v>270</v>
@@ -3215,16 +3215,16 @@
         <v>0</v>
       </c>
       <c r="J39" s="1">
-        <v>578</v>
+        <v>434</v>
       </c>
       <c r="K39" s="1">
-        <v>2123</v>
+        <v>2625</v>
       </c>
       <c r="L39" s="14">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="M39" s="1">
-        <v>776</v>
+        <v>1</v>
       </c>
       <c r="N39" s="1">
         <v>1105</v>
@@ -3259,16 +3259,16 @@
         <v>0</v>
       </c>
       <c r="J40" s="5">
-        <v>108</v>
+        <v>135</v>
       </c>
       <c r="K40" s="5">
-        <v>3921</v>
+        <v>4619</v>
       </c>
       <c r="L40" s="18">
-        <v>73</v>
+        <v>5</v>
       </c>
       <c r="M40" s="5">
-        <v>602</v>
+        <v>0</v>
       </c>
       <c r="N40" s="5">
         <v>181</v>
@@ -3303,16 +3303,16 @@
         <v>0</v>
       </c>
       <c r="J41" s="5">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="K41" s="5">
-        <v>16624</v>
+        <v>17642</v>
       </c>
       <c r="L41" s="18">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="M41" s="5">
-        <v>935</v>
+        <v>1</v>
       </c>
       <c r="N41" s="5">
         <v>555</v>
@@ -3347,16 +3347,16 @@
         <v>0</v>
       </c>
       <c r="J42" s="5">
-        <v>346</v>
+        <v>379</v>
       </c>
       <c r="K42" s="5">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="L42" s="18">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="M42" s="5">
-        <v>190</v>
+        <v>0</v>
       </c>
       <c r="N42" s="5">
         <v>79</v>
@@ -3391,16 +3391,16 @@
         <v>0</v>
       </c>
       <c r="J43" s="5">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="K43" s="5">
-        <v>1428</v>
+        <v>1406</v>
       </c>
       <c r="L43" s="18">
         <v>0</v>
       </c>
       <c r="M43" s="5">
-        <v>152</v>
+        <v>0</v>
       </c>
       <c r="N43" s="5">
         <v>134</v>
@@ -3435,16 +3435,16 @@
         <v>0</v>
       </c>
       <c r="J44" s="5">
-        <v>643</v>
+        <v>41</v>
       </c>
       <c r="K44" s="5">
-        <v>2744</v>
+        <v>998</v>
       </c>
       <c r="L44" s="18">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="M44" s="5">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="N44" s="5">
         <v>7</v>
@@ -3479,16 +3479,16 @@
         <v>0</v>
       </c>
       <c r="J45" s="1">
-        <v>1793</v>
+        <v>2098</v>
       </c>
       <c r="K45" s="1">
-        <v>1747</v>
+        <v>1379</v>
       </c>
       <c r="L45" s="14">
-        <v>1781</v>
+        <v>2044</v>
       </c>
       <c r="M45" s="1">
-        <v>1527</v>
+        <v>2</v>
       </c>
       <c r="N45" s="1">
         <v>739</v>
@@ -3523,16 +3523,16 @@
         <v>0</v>
       </c>
       <c r="J46" s="2">
-        <v>10107</v>
+        <v>9958</v>
       </c>
       <c r="K46" s="2">
-        <v>9883</v>
+        <v>10376</v>
       </c>
       <c r="L46" s="15">
-        <v>478</v>
+        <v>44</v>
       </c>
       <c r="M46" s="2">
-        <v>5840</v>
+        <v>458</v>
       </c>
       <c r="N46" s="2">
         <v>3647</v>
@@ -3567,16 +3567,16 @@
         <v>587</v>
       </c>
       <c r="J47" s="1">
-        <v>12891</v>
+        <v>12387</v>
       </c>
       <c r="K47" s="1">
-        <v>35108</v>
+        <v>36684</v>
       </c>
       <c r="L47" s="14">
-        <v>1217</v>
+        <v>1021</v>
       </c>
       <c r="M47" s="1">
-        <v>5711</v>
+        <v>296</v>
       </c>
       <c r="N47" s="1">
         <v>7191</v>
@@ -3611,16 +3611,16 @@
         <v>58</v>
       </c>
       <c r="J48" s="2">
-        <v>9122</v>
+        <v>9542</v>
       </c>
       <c r="K48" s="2">
-        <v>14136</v>
+        <v>14093</v>
       </c>
       <c r="L48" s="15">
-        <v>37</v>
+        <v>87</v>
       </c>
       <c r="M48" s="2">
-        <v>5707</v>
+        <v>0</v>
       </c>
       <c r="N48" s="2">
         <v>2134</v>
@@ -3655,16 +3655,16 @@
         <v>162</v>
       </c>
       <c r="J49" s="1">
-        <v>5785</v>
+        <v>5887</v>
       </c>
       <c r="K49" s="1">
-        <v>11235</v>
+        <v>12024</v>
       </c>
       <c r="L49" s="14">
-        <v>988</v>
+        <v>552</v>
       </c>
       <c r="M49" s="1">
-        <v>2116</v>
+        <v>165</v>
       </c>
       <c r="N49" s="1">
         <v>3051</v>
@@ -3699,16 +3699,16 @@
         <v>0</v>
       </c>
       <c r="J50" s="2">
-        <v>18075</v>
+        <v>22025</v>
       </c>
       <c r="K50" s="2">
-        <v>24148</v>
+        <v>25535</v>
       </c>
       <c r="L50" s="15">
-        <v>3986</v>
+        <v>3743</v>
       </c>
       <c r="M50" s="2">
-        <v>4890</v>
+        <v>708</v>
       </c>
       <c r="N50" s="2">
         <v>8046</v>
@@ -3743,16 +3743,16 @@
         <v>0</v>
       </c>
       <c r="J51" s="1">
-        <v>3843</v>
+        <v>4080</v>
       </c>
       <c r="K51" s="1">
-        <v>2728</v>
+        <v>3779</v>
       </c>
       <c r="L51" s="14">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="M51" s="1">
-        <v>1229</v>
+        <v>0</v>
       </c>
       <c r="N51" s="1">
         <v>1930</v>
@@ -3787,16 +3787,16 @@
         <v>0</v>
       </c>
       <c r="J52" s="2">
-        <v>8370</v>
+        <v>8248</v>
       </c>
       <c r="K52" s="2">
-        <v>13427</v>
+        <v>13044</v>
       </c>
       <c r="L52" s="15">
-        <v>1221</v>
+        <v>656</v>
       </c>
       <c r="M52" s="2">
-        <v>4751</v>
+        <v>2</v>
       </c>
       <c r="N52" s="2">
         <v>3971</v>
@@ -3831,16 +3831,16 @@
         <v>0</v>
       </c>
       <c r="J53" s="1">
-        <v>2510</v>
+        <v>2214</v>
       </c>
       <c r="K53" s="1">
-        <v>1041</v>
+        <v>1058</v>
       </c>
       <c r="L53" s="14">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="M53" s="1">
-        <v>2218</v>
+        <v>0</v>
       </c>
       <c r="N53" s="1">
         <v>1238</v>
@@ -3875,16 +3875,16 @@
         <v>0</v>
       </c>
       <c r="J54" s="2">
-        <v>1222</v>
+        <v>1510</v>
       </c>
       <c r="K54" s="2">
-        <v>2162</v>
+        <v>2094</v>
       </c>
       <c r="L54" s="15">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="M54" s="2">
-        <v>2066</v>
+        <v>0</v>
       </c>
       <c r="N54" s="2">
         <v>225</v>
@@ -3919,16 +3919,16 @@
         <v>0</v>
       </c>
       <c r="J55" s="1">
-        <v>2786</v>
+        <v>2874</v>
       </c>
       <c r="K55" s="1">
-        <v>2439</v>
+        <v>4032</v>
       </c>
       <c r="L55" s="14">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="M55" s="1">
-        <v>1765</v>
+        <v>3</v>
       </c>
       <c r="N55" s="1">
         <v>2308</v>
@@ -3972,19 +3972,19 @@
       </c>
       <c r="J56" s="20">
         <f t="shared" si="0"/>
-        <v>11695</v>
+        <v>10978</v>
       </c>
       <c r="K56" s="20">
         <f t="shared" si="0"/>
-        <v>8688</v>
+        <v>8550</v>
       </c>
       <c r="L56" s="20">
         <f t="shared" si="0"/>
-        <v>2026</v>
+        <v>835</v>
       </c>
       <c r="M56" s="20">
         <f t="shared" si="0"/>
-        <v>7769</v>
+        <v>516</v>
       </c>
       <c r="N56" s="20">
         <f t="shared" si="0"/>
@@ -4029,19 +4029,19 @@
       </c>
       <c r="J57" s="22">
         <f t="shared" si="2"/>
-        <v>1186</v>
+        <v>688</v>
       </c>
       <c r="K57" s="22">
         <f t="shared" si="2"/>
-        <v>24768</v>
+        <v>24709</v>
       </c>
       <c r="L57" s="22">
         <f t="shared" si="2"/>
-        <v>176</v>
+        <v>55</v>
       </c>
       <c r="M57" s="22">
         <f t="shared" si="2"/>
-        <v>1893</v>
+        <v>1</v>
       </c>
       <c r="N57" s="22">
         <f t="shared" si="2"/>
@@ -4086,19 +4086,19 @@
       </c>
       <c r="J58" s="21">
         <f t="shared" si="4"/>
-        <v>457234</v>
+        <v>458444</v>
       </c>
       <c r="K58" s="21">
         <f t="shared" si="4"/>
-        <v>573667</v>
+        <v>612035</v>
       </c>
       <c r="L58" s="21">
         <f t="shared" si="4"/>
-        <v>42383</v>
+        <v>32014</v>
       </c>
       <c r="M58" s="21">
         <f t="shared" si="4"/>
-        <v>170301</v>
+        <v>5623</v>
       </c>
       <c r="N58" s="21">
         <f t="shared" si="4"/>

</xml_diff>